<commit_message>
add arima call via threads
</commit_message>
<xml_diff>
--- a/dataset/cpu - Copy.xlsx
+++ b/dataset/cpu - Copy.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I851169\source\repos\dev\autoscaling\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6CF7FC-C79A-4A6F-A39F-A921C23B0BED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63847A7-1DA3-400F-992B-9FD95DBFF22B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="241">
   <si>
     <t>date</t>
   </si>
@@ -743,33 +743,6 @@
   </si>
   <si>
     <t>04/26/2021 00:19:50</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:22:34</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:22:35</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:25:12</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:25:13</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:27:51</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:27:52</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:30:24</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:33:01</t>
-  </si>
-  <si>
-    <t>04/26/2021 00:33:02</t>
   </si>
 </sst>
 </file>
@@ -808,10 +781,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,16 +1086,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B519"/>
+  <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A490" workbookViewId="0">
-      <selection activeCell="F513" sqref="F513"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3074,7 +3043,7 @@
         <v>237</v>
       </c>
       <c r="B244">
-        <v>94.098399999999998</v>
+        <v>38</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,7 +3051,7 @@
         <v>238</v>
       </c>
       <c r="B245">
-        <v>95.423699999999997</v>
+        <v>47</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -3090,7 +3059,7 @@
         <v>239</v>
       </c>
       <c r="B246">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3098,2183 +3067,7 @@
         <v>240</v>
       </c>
       <c r="B247">
-        <v>92.333299999999994</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>241</v>
-      </c>
-      <c r="B248">
-        <v>78.333299999999994</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>242</v>
-      </c>
-      <c r="B249">
-        <v>34.406799999999997</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>243</v>
-      </c>
-      <c r="B250">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>244</v>
-      </c>
-      <c r="B251">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>245</v>
-      </c>
-      <c r="B252">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>246</v>
-      </c>
-      <c r="B253">
-        <v>75.423699999999997</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>247</v>
-      </c>
-      <c r="B254">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>247</v>
-      </c>
-      <c r="B255">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>248</v>
-      </c>
-      <c r="B256">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>249</v>
-      </c>
-      <c r="B257">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2">
-        <v>44312.022638888891</v>
-      </c>
-      <c r="B258">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2">
-        <v>44312.02847222222</v>
-      </c>
-      <c r="B259">
-        <v>26.333300000000001</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="2">
-        <v>44312.029861111114</v>
-      </c>
-      <c r="B260">
-        <v>97.704899999999995</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2">
-        <v>44312.031250057873</v>
-      </c>
-      <c r="B261">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2">
-        <v>44312.032639004632</v>
-      </c>
-      <c r="B262">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2">
-        <v>44312.034027951391</v>
-      </c>
-      <c r="B263">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2">
-        <v>44312.03541689815</v>
-      </c>
-      <c r="B264">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
-        <v>44312.036805844909</v>
-      </c>
-      <c r="B265">
-        <v>0.49180000000000001</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2">
-        <v>44312.038194791669</v>
-      </c>
-      <c r="B266">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2">
-        <v>44312.039583738428</v>
-      </c>
-      <c r="B267">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2">
-        <v>44312.040972685187</v>
-      </c>
-      <c r="B268">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2">
-        <v>44312.042361631946</v>
-      </c>
-      <c r="B269">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2">
-        <v>44312.043750578705</v>
-      </c>
-      <c r="B270">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2">
-        <v>44312.045139525464</v>
-      </c>
-      <c r="B271">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2">
-        <v>44312.046528472223</v>
-      </c>
-      <c r="B272">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2">
-        <v>44312.047917418982</v>
-      </c>
-      <c r="B273">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
-        <v>44312.049306365741</v>
-      </c>
-      <c r="B274">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
-        <v>44312.0506953125</v>
-      </c>
-      <c r="B275">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
-        <v>44312.05208425926</v>
-      </c>
-      <c r="B276">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="2">
-        <v>44312.053473206019</v>
-      </c>
-      <c r="B277">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2">
-        <v>44312.054862152778</v>
-      </c>
-      <c r="B278">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="2">
-        <v>44312.056251099537</v>
-      </c>
-      <c r="B279">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
-        <v>44312.057640046296</v>
-      </c>
-      <c r="B280">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
-        <v>44312.059028993055</v>
-      </c>
-      <c r="B281">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
-        <v>44312.060417939814</v>
-      </c>
-      <c r="B282">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
-        <v>44312.061806886573</v>
-      </c>
-      <c r="B283">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
-        <v>44312.063195833332</v>
-      </c>
-      <c r="B284">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="2">
-        <v>44312.064584780092</v>
-      </c>
-      <c r="B285">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="2">
-        <v>44312.065973726851</v>
-      </c>
-      <c r="B286">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2">
-        <v>44312.06736267361</v>
-      </c>
-      <c r="B287">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="2">
-        <v>44312.068751620369</v>
-      </c>
-      <c r="B288">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
-        <v>44312.070140567128</v>
-      </c>
-      <c r="B289">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
-        <v>44312.071529513887</v>
-      </c>
-      <c r="B290">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
-        <v>44312.072918460646</v>
-      </c>
-      <c r="B291">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
-        <v>44312.074307407405</v>
-      </c>
-      <c r="B292">
-        <v>30.983599999999999</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
-        <v>44312.075696354164</v>
-      </c>
-      <c r="B293">
-        <v>17.666699999999999</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
-        <v>44312.077085300923</v>
-      </c>
-      <c r="B294">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
-        <v>44312.078474247683</v>
-      </c>
-      <c r="B295">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
-        <v>44312.079863194442</v>
-      </c>
-      <c r="B296">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
-        <v>44312.081252141201</v>
-      </c>
-      <c r="B297">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
-        <v>44312.08264108796</v>
-      </c>
-      <c r="B298">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="2">
-        <v>44312.084030034719</v>
-      </c>
-      <c r="B299">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="2">
-        <v>44312.085418981478</v>
-      </c>
-      <c r="B300">
-        <v>81.186400000000006</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="2">
-        <v>44312.086807928237</v>
-      </c>
-      <c r="B301">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
-        <v>44312.088196875004</v>
-      </c>
-      <c r="B302">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
-        <v>44312.089585821763</v>
-      </c>
-      <c r="B303">
-        <v>80.819699999999997</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
-        <v>44312.090974768522</v>
-      </c>
-      <c r="B304">
-        <v>83.666700000000006</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="2">
-        <v>44312.092363715281</v>
-      </c>
-      <c r="B305">
-        <v>99.666700000000006</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="2">
-        <v>44312.09375266204</v>
-      </c>
-      <c r="B306">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="2">
-        <v>44312.095141608799</v>
-      </c>
-      <c r="B307">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="2">
-        <v>44312.096530555558</v>
-      </c>
-      <c r="B308">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="2">
-        <v>44312.097919502317</v>
-      </c>
-      <c r="B309">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="2">
-        <v>44312.099308449076</v>
-      </c>
-      <c r="B310">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="2">
-        <v>44312.100697395836</v>
-      </c>
-      <c r="B311">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="2">
-        <v>44312.102086342595</v>
-      </c>
-      <c r="B312">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="2">
-        <v>44312.103475289354</v>
-      </c>
-      <c r="B313">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="2">
-        <v>44312.104864236113</v>
-      </c>
-      <c r="B314">
-        <v>20.666699999999999</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="2">
-        <v>44312.106253182872</v>
-      </c>
-      <c r="B315">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="2">
-        <v>44312.107642129631</v>
-      </c>
-      <c r="B316">
-        <v>83.833299999999994</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="2">
-        <v>44312.10903107639</v>
-      </c>
-      <c r="B317">
-        <v>91.016900000000007</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="2">
-        <v>44312.110420023149</v>
-      </c>
-      <c r="B318">
-        <v>83.333299999999994</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="2">
-        <v>44312.111808969908</v>
-      </c>
-      <c r="B319">
-        <v>42.7119</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="2">
-        <v>44312.113197916668</v>
-      </c>
-      <c r="B320">
-        <v>56.833300000000001</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="2">
-        <v>44312.114586863427</v>
-      </c>
-      <c r="B321">
-        <v>64.827600000000004</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="2">
-        <v>44312.115975810186</v>
-      </c>
-      <c r="B322">
-        <v>37.627099999999999</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="2">
-        <v>44312.117364756945</v>
-      </c>
-      <c r="B323">
-        <v>79.833299999999994</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="2">
-        <v>44312.118753703704</v>
-      </c>
-      <c r="B324">
-        <v>99.836100000000002</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="2">
-        <v>44312.120142650463</v>
-      </c>
-      <c r="B325">
-        <v>62.5</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="2">
-        <v>44312.121531597222</v>
-      </c>
-      <c r="B326">
-        <v>35.932200000000002</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="2">
-        <v>44312.122920543981</v>
-      </c>
-      <c r="B327">
-        <v>61.639299999999999</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="2">
-        <v>44312.12430949074</v>
-      </c>
-      <c r="B328">
-        <v>41.355899999999998</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="2">
-        <v>44312.1256984375</v>
-      </c>
-      <c r="B329">
-        <v>2.2951000000000001</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="2">
-        <v>44312.127087384259</v>
-      </c>
-      <c r="B330">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="2">
-        <v>44312.128476331018</v>
-      </c>
-      <c r="B331">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="2">
-        <v>44312.129865277777</v>
-      </c>
-      <c r="B332">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2">
-        <v>44312.131254224536</v>
-      </c>
-      <c r="B333">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="2">
-        <v>44312.132643171295</v>
-      </c>
-      <c r="B334">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="2">
-        <v>44312.134032118054</v>
-      </c>
-      <c r="B335">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="2">
-        <v>44312.135421064813</v>
-      </c>
-      <c r="B336">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="2">
-        <v>44312.136810011572</v>
-      </c>
-      <c r="B337">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="2">
-        <v>44312.138198958331</v>
-      </c>
-      <c r="B338">
-        <v>99.836100000000002</v>
-      </c>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="2">
-        <v>44312.139587905091</v>
-      </c>
-      <c r="B339">
-        <v>81.186400000000006</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="2">
-        <v>44312.14097685185</v>
-      </c>
-      <c r="B340">
-        <v>79.322000000000003</v>
-      </c>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="2">
-        <v>44312.142365798609</v>
-      </c>
-      <c r="B341">
-        <v>41.666699999999999</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="2">
-        <v>44312.143754745368</v>
-      </c>
-      <c r="B342">
-        <v>38.333300000000001</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="2">
-        <v>44312.145143692127</v>
-      </c>
-      <c r="B343">
-        <v>63.389800000000001</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="2">
-        <v>44312.146532638886</v>
-      </c>
-      <c r="B344">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="2">
-        <v>44312.147921585645</v>
-      </c>
-      <c r="B345">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="2">
-        <v>44312.149310532404</v>
-      </c>
-      <c r="B346">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" s="2">
-        <v>44312.150699479163</v>
-      </c>
-      <c r="B347">
-        <v>0.50849999999999995</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" s="2">
-        <v>44312.152088425923</v>
-      </c>
-      <c r="B348">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" s="2">
-        <v>44312.153477372682</v>
-      </c>
-      <c r="B349">
-        <v>0.49180000000000001</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" s="2">
-        <v>44312.154866319448</v>
-      </c>
-      <c r="B350">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" s="2">
-        <v>44312.156255266207</v>
-      </c>
-      <c r="B351">
-        <v>0.50849999999999995</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" s="2">
-        <v>44312.157644212966</v>
-      </c>
-      <c r="B352">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A353" s="2">
-        <v>44312.159033159725</v>
-      </c>
-      <c r="B353">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" s="2">
-        <v>44312.160422106484</v>
-      </c>
-      <c r="B354">
-        <v>63.166699999999999</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" s="2">
-        <v>44312.161811053244</v>
-      </c>
-      <c r="B355">
-        <v>61.666699999999999</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A356" s="2">
-        <v>44312.163200000003</v>
-      </c>
-      <c r="B356">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A357" s="2">
-        <v>44312.164588946762</v>
-      </c>
-      <c r="B357">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" s="2">
-        <v>44312.165977893521</v>
-      </c>
-      <c r="B358">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" s="2">
-        <v>44312.16736684028</v>
-      </c>
-      <c r="B359">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" s="2">
-        <v>44312.168755787039</v>
-      </c>
-      <c r="B360">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" s="2">
-        <v>44312.170144733798</v>
-      </c>
-      <c r="B361">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" s="2">
-        <v>44312.171533680557</v>
-      </c>
-      <c r="B362">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="2">
-        <v>44312.172922627316</v>
-      </c>
-      <c r="B363">
-        <v>48.333300000000001</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" s="2">
-        <v>44312.174311574076</v>
-      </c>
-      <c r="B364">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="2">
-        <v>44312.175700520835</v>
-      </c>
-      <c r="B365">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="2">
-        <v>44312.177089467594</v>
-      </c>
-      <c r="B366">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A367" s="2">
-        <v>44312.178478414353</v>
-      </c>
-      <c r="B367">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A368" s="2">
-        <v>44312.179867361112</v>
-      </c>
-      <c r="B368">
-        <v>49.152500000000003</v>
-      </c>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="2">
-        <v>44312.181256307871</v>
-      </c>
-      <c r="B369">
-        <v>82.833299999999994</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="2">
-        <v>44312.18264525463</v>
-      </c>
-      <c r="B370">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="2">
-        <v>44312.184034201389</v>
-      </c>
-      <c r="B371">
-        <v>71.166700000000006</v>
-      </c>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="2">
-        <v>44312.185423148148</v>
-      </c>
-      <c r="B372">
-        <v>77.540999999999997</v>
-      </c>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="2">
-        <v>44312.186812094908</v>
-      </c>
-      <c r="B373">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="2">
-        <v>44312.188201041667</v>
-      </c>
-      <c r="B374">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="2">
-        <v>44312.189589988426</v>
-      </c>
-      <c r="B375">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="2">
-        <v>44312.190978935185</v>
-      </c>
-      <c r="B376">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="2">
-        <v>44312.192367881944</v>
-      </c>
-      <c r="B377">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="2">
-        <v>44312.193756828703</v>
-      </c>
-      <c r="B378">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="2">
-        <v>44312.195145775462</v>
-      </c>
-      <c r="B379">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="2">
-        <v>44312.196534722221</v>
-      </c>
-      <c r="B380">
-        <v>8.1667000000000005</v>
-      </c>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="2">
-        <v>44312.19792366898</v>
-      </c>
-      <c r="B381">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="2">
-        <v>44312.199312615739</v>
-      </c>
-      <c r="B382">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="2">
-        <v>44312.200701562499</v>
-      </c>
-      <c r="B383">
-        <v>99.5</v>
-      </c>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="2">
-        <v>44312.202090509258</v>
-      </c>
-      <c r="B384">
-        <v>93.770499999999998</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="2">
-        <v>44312.203479456017</v>
-      </c>
-      <c r="B385">
-        <v>99.180300000000003</v>
-      </c>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="2">
-        <v>44312.204868402776</v>
-      </c>
-      <c r="B386">
-        <v>47.166699999999999</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="2">
-        <v>44312.206257349535</v>
-      </c>
-      <c r="B387">
-        <v>63.389800000000001</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="2">
-        <v>44312.207646296294</v>
-      </c>
-      <c r="B388">
-        <v>38.1967</v>
-      </c>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="2">
-        <v>44312.209035243053</v>
-      </c>
-      <c r="B389">
-        <v>60.333300000000001</v>
-      </c>
-    </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="2">
-        <v>44312.210424189812</v>
-      </c>
-      <c r="B390">
-        <v>48.064500000000002</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="2">
-        <v>44312.211813136571</v>
-      </c>
-      <c r="B391">
-        <v>51.666699999999999</v>
-      </c>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="2">
-        <v>44312.213202083331</v>
-      </c>
-      <c r="B392">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="2">
-        <v>44312.21459103009</v>
-      </c>
-      <c r="B393">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="2">
-        <v>44312.215979976849</v>
-      </c>
-      <c r="B394">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="2">
-        <v>44312.217368923608</v>
-      </c>
-      <c r="B395">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="2">
-        <v>44312.218757870367</v>
-      </c>
-      <c r="B396">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="2">
-        <v>44312.220146817126</v>
-      </c>
-      <c r="B397">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="2">
-        <v>44312.221535763892</v>
-      </c>
-      <c r="B398">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="2">
-        <v>44312.222924710652</v>
-      </c>
-      <c r="B399">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="2">
-        <v>44312.224313657411</v>
-      </c>
-      <c r="B400">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="2">
-        <v>44312.22570260417</v>
-      </c>
-      <c r="B401">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="2">
-        <v>44312.227091550929</v>
-      </c>
-      <c r="B402">
-        <v>91.333299999999994</v>
-      </c>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="2">
-        <v>44312.228480497688</v>
-      </c>
-      <c r="B403">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="2">
-        <v>44312.229869444447</v>
-      </c>
-      <c r="B404">
-        <v>98.833299999999994</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="2">
-        <v>44312.231258391206</v>
-      </c>
-      <c r="B405">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="2">
-        <v>44312.232647337965</v>
-      </c>
-      <c r="B406">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="2">
-        <v>44312.234036284724</v>
-      </c>
-      <c r="B407">
-        <v>0.66669999999999996</v>
-      </c>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="2">
-        <v>44312.235425231484</v>
-      </c>
-      <c r="B408">
-        <v>0.50849999999999995</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="2">
-        <v>44312.236814178243</v>
-      </c>
-      <c r="B409">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="2">
-        <v>44312.238203125002</v>
-      </c>
-      <c r="B410">
-        <v>0.16389999999999999</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="2">
-        <v>44312.239592071761</v>
-      </c>
-      <c r="B411">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="2">
-        <v>44312.24098101852</v>
-      </c>
-      <c r="B412">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="2">
-        <v>44312.242369965279</v>
-      </c>
-      <c r="B413">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="2">
-        <v>44312.243758912038</v>
-      </c>
-      <c r="B414">
-        <v>61.166699999999999</v>
-      </c>
-    </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="2">
-        <v>44312.245147858797</v>
-      </c>
-      <c r="B415">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="2">
-        <v>44312.246536805556</v>
-      </c>
-      <c r="B416">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A417" s="2">
-        <v>44312.247925752315</v>
-      </c>
-      <c r="B417">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A418" s="2">
-        <v>44312.249314699075</v>
-      </c>
-      <c r="B418">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A419" s="2">
-        <v>44312.250703645834</v>
-      </c>
-      <c r="B419">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A420" s="2">
-        <v>44312.252092592593</v>
-      </c>
-      <c r="B420">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A421" s="2">
-        <v>44312.253481539352</v>
-      </c>
-      <c r="B421">
-        <v>0.16389999999999999</v>
-      </c>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A422" s="2">
-        <v>44312.254870486111</v>
-      </c>
-      <c r="B422">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A423" s="2">
-        <v>44312.25625943287</v>
-      </c>
-      <c r="B423">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A424" s="2">
-        <v>44312.257648379629</v>
-      </c>
-      <c r="B424">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A425" s="2">
-        <v>44312.259037326388</v>
-      </c>
-      <c r="B425">
-        <v>0.16389999999999999</v>
-      </c>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A426" s="2">
-        <v>44312.260426273147</v>
-      </c>
-      <c r="B426">
-        <v>0.16389999999999999</v>
-      </c>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A427" s="2">
-        <v>44312.261815219907</v>
-      </c>
-      <c r="B427">
-        <v>0.16950000000000001</v>
-      </c>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A428" s="2">
-        <v>44312.263204166666</v>
-      </c>
-      <c r="B428">
-        <v>61.694899999999997</v>
-      </c>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A429" s="2">
-        <v>44312.264593113425</v>
-      </c>
-      <c r="B429">
-        <v>81.639300000000006</v>
-      </c>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A430" s="2">
-        <v>44312.265982060184</v>
-      </c>
-      <c r="B430">
-        <v>96.666700000000006</v>
-      </c>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A431" s="2">
-        <v>44312.267371006943</v>
-      </c>
-      <c r="B431">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A432" s="2">
-        <v>44312.268759953702</v>
-      </c>
-      <c r="B432">
-        <v>0.16389999999999999</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="2">
-        <v>44312.270148900461</v>
-      </c>
-      <c r="B433">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="2">
-        <v>44312.27153784722</v>
-      </c>
-      <c r="B434">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="2">
-        <v>44312.272926793979</v>
-      </c>
-      <c r="B435">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="2">
-        <v>44312.274315740739</v>
-      </c>
-      <c r="B436">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="2">
-        <v>44312.275704687498</v>
-      </c>
-      <c r="B437">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="2">
-        <v>44312.277093634257</v>
-      </c>
-      <c r="B438">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A439" s="2">
-        <v>44312.278482581016</v>
-      </c>
-      <c r="B439">
-        <v>0.16389999999999999</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A440" s="2">
-        <v>44312.279871527775</v>
-      </c>
-      <c r="B440">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A441" s="2">
-        <v>44312.281260474534</v>
-      </c>
-      <c r="B441">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A442" s="2">
-        <v>44312.282649421293</v>
-      </c>
-      <c r="B442">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A443" s="2">
-        <v>44312.284038368052</v>
-      </c>
-      <c r="B443">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A444" s="2">
-        <v>44312.285427314811</v>
-      </c>
-      <c r="B444">
-        <v>97.118600000000001</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A445" s="2">
-        <v>44312.28681626157</v>
-      </c>
-      <c r="B445">
-        <v>94.666700000000006</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" s="2">
-        <v>44312.288205208337</v>
-      </c>
-      <c r="B446">
-        <v>99.333299999999994</v>
-      </c>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A447" s="2">
-        <v>44312.289594155096</v>
-      </c>
-      <c r="B447">
-        <v>61.311500000000002</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" s="2">
-        <v>44312.290983101855</v>
-      </c>
-      <c r="B448">
-        <v>34.406799999999997</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" s="2">
-        <v>44312.292372048614</v>
-      </c>
-      <c r="B449">
-        <v>48.166699999999999</v>
-      </c>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A450" s="2">
-        <v>44312.293760995373</v>
-      </c>
-      <c r="B450">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A451" s="2">
-        <v>44312.295149942132</v>
-      </c>
-      <c r="B451">
-        <v>99.166700000000006</v>
-      </c>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A452" s="2">
-        <v>44312.296538888892</v>
-      </c>
-      <c r="B452">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A453" s="2">
-        <v>44312.297927835651</v>
-      </c>
-      <c r="B453">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A454" s="2">
-        <v>44312.29931678241</v>
-      </c>
-      <c r="B454">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A455" s="2">
-        <v>44312.300705729169</v>
-      </c>
-      <c r="B455">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A456" s="2">
-        <v>44312.302094675928</v>
-      </c>
-      <c r="B456">
-        <v>0.83330000000000004</v>
-      </c>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A457" s="2">
-        <v>44312.303483622687</v>
-      </c>
-      <c r="B457">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A458" s="2">
-        <v>44312.304872569446</v>
-      </c>
-      <c r="B458">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A459" s="2">
-        <v>44312.306261516205</v>
-      </c>
-      <c r="B459">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A460" s="2">
-        <v>44312.307650462964</v>
-      </c>
-      <c r="B460">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A461" s="2">
-        <v>44312.309039409723</v>
-      </c>
-      <c r="B461">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A462" s="2">
-        <v>44312.310428356483</v>
-      </c>
-      <c r="B462">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A463" s="2">
-        <v>44312.311817303242</v>
-      </c>
-      <c r="B463">
-        <v>0.49180000000000001</v>
-      </c>
-    </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A464" s="2">
-        <v>44312.313206250001</v>
-      </c>
-      <c r="B464">
-        <v>0.49180000000000001</v>
-      </c>
-    </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A465" s="2">
-        <v>44312.31459519676</v>
-      </c>
-      <c r="B465">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A466" s="2">
-        <v>44312.315984143519</v>
-      </c>
-      <c r="B466">
-        <v>0.3226</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A467" s="2">
-        <v>44312.317373090278</v>
-      </c>
-      <c r="B467">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A468" s="2">
-        <v>44312.318762037037</v>
-      </c>
-      <c r="B468">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A469" s="2">
-        <v>44312.320150983796</v>
-      </c>
-      <c r="B469">
-        <v>99.333299999999994</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A470" s="2">
-        <v>44312.321539930555</v>
-      </c>
-      <c r="B470">
-        <v>80.5</v>
-      </c>
-    </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A471" s="2">
-        <v>44312.322928877315</v>
-      </c>
-      <c r="B471">
-        <v>99.666700000000006</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A472" s="2">
-        <v>44312.324317824074</v>
-      </c>
-      <c r="B472">
-        <v>91.475399999999993</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A473" s="2">
-        <v>44312.325706770833</v>
-      </c>
-      <c r="B473">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A474" s="2">
-        <v>44312.327095717592</v>
-      </c>
-      <c r="B474">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A475" s="2">
-        <v>44312.328484664351</v>
-      </c>
-      <c r="B475">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A476" s="2">
-        <v>44312.32987361111</v>
-      </c>
-      <c r="B476">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A477" s="2">
-        <v>44312.331262557869</v>
-      </c>
-      <c r="B477">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A478" s="2">
-        <v>44312.332651504628</v>
-      </c>
-      <c r="B478">
-        <v>0.4839</v>
-      </c>
-    </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A479" s="2">
-        <v>44312.334040451387</v>
-      </c>
-      <c r="B479">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A480" s="2">
-        <v>44312.335429398147</v>
-      </c>
-      <c r="B480">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A481" s="2">
-        <v>44312.336818344906</v>
-      </c>
-      <c r="B481">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A482" s="2">
-        <v>44312.338207291665</v>
-      </c>
-      <c r="B482">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A483" s="2">
-        <v>44312.339596238424</v>
-      </c>
-      <c r="B483">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A484" s="2">
-        <v>44312.340985185183</v>
-      </c>
-      <c r="B484">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A485" s="2">
-        <v>44312.342374131942</v>
-      </c>
-      <c r="B485">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A486" s="2">
-        <v>44312.343763078701</v>
-      </c>
-      <c r="B486">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A487" s="2">
-        <v>44312.34515202546</v>
-      </c>
-      <c r="B487">
-        <v>0.66669999999999996</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A488" s="2">
-        <v>44312.346540972219</v>
-      </c>
-      <c r="B488">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A489" s="2">
-        <v>44312.347929918978</v>
-      </c>
-      <c r="B489">
-        <v>85.762699999999995</v>
-      </c>
-    </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A490" s="2">
-        <v>44312.349318865738</v>
-      </c>
-      <c r="B490">
-        <v>82.666700000000006</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A491" s="2">
-        <v>44312.350707812497</v>
-      </c>
-      <c r="B491">
-        <v>80.833299999999994</v>
-      </c>
-    </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A492" s="2">
-        <v>44312.352096759256</v>
-      </c>
-      <c r="B492">
-        <v>80.169499999999999</v>
-      </c>
-    </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A493" s="2">
-        <v>44312.353485706015</v>
-      </c>
-      <c r="B493">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A494" s="2">
-        <v>44312.354874652781</v>
-      </c>
-      <c r="B494">
-        <v>48.333300000000001</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A495" s="2">
-        <v>44312.35626359954</v>
-      </c>
-      <c r="B495">
-        <v>19.333300000000001</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A496" s="2">
-        <v>44312.3576525463</v>
-      </c>
-      <c r="B496">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A497" s="2">
-        <v>44312.359041493059</v>
-      </c>
-      <c r="B497">
-        <v>0.49180000000000001</v>
-      </c>
-    </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A498" s="2">
-        <v>44312.360430439818</v>
-      </c>
-      <c r="B498">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A499" s="2">
-        <v>44312.361819386577</v>
-      </c>
-      <c r="B499">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A500" s="2">
-        <v>44312.363208333336</v>
-      </c>
-      <c r="B500">
-        <v>0.32790000000000002</v>
-      </c>
-    </row>
-    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A501" s="2">
-        <v>44312.364597280095</v>
-      </c>
-      <c r="B501">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A502" s="2">
-        <v>44312.365986226854</v>
-      </c>
-      <c r="B502">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A503" s="2">
-        <v>44312.367375173613</v>
-      </c>
-      <c r="B503">
-        <v>94.098399999999998</v>
-      </c>
-    </row>
-    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A504" s="2">
-        <v>44312.368764120372</v>
-      </c>
-      <c r="B504">
-        <v>95.423699999999997</v>
-      </c>
-    </row>
-    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A505" s="2">
-        <v>44312.370153067131</v>
-      </c>
-      <c r="B505">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A506" s="2">
-        <v>44312.371542013891</v>
-      </c>
-      <c r="B506">
-        <v>92.333299999999994</v>
-      </c>
-    </row>
-    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A507" s="2">
-        <v>44312.37293096065</v>
-      </c>
-      <c r="B507">
-        <v>78.333299999999994</v>
-      </c>
-    </row>
-    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A508" s="2">
-        <v>44312.374319907409</v>
-      </c>
-      <c r="B508">
-        <v>34.406799999999997</v>
-      </c>
-    </row>
-    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A509" s="2">
-        <v>44312.375708854168</v>
-      </c>
-      <c r="B509">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A510" s="2">
-        <v>44312.377097800927</v>
-      </c>
-      <c r="B510">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A511" s="2">
-        <v>44312.378486747686</v>
-      </c>
-      <c r="B511">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A512" s="2">
-        <v>44312.379875694445</v>
-      </c>
-      <c r="B512">
-        <v>75.423699999999997</v>
-      </c>
-    </row>
-    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A513" s="2">
-        <v>44312.381264641204</v>
-      </c>
-      <c r="B513">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A514" s="2">
-        <v>44312.382653587963</v>
-      </c>
-      <c r="B514">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A515" s="2">
-        <v>44312.384042534723</v>
-      </c>
-      <c r="B515">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A516" s="2">
-        <v>44312.385431481482</v>
-      </c>
-      <c r="B516">
-        <v>0.16669999999999999</v>
-      </c>
-    </row>
-    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A517" s="2">
-        <v>44312.386820428241</v>
-      </c>
-      <c r="B517">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A518" s="2">
-        <v>44312.388209375</v>
-      </c>
-      <c r="B518">
-        <v>26.333300000000001</v>
-      </c>
-    </row>
-    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A519" s="2">
-        <v>44312.389598321759</v>
-      </c>
-      <c r="B519">
-        <v>97.704899999999995</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>